<commit_message>
Add backlog and prod report with SAT reference
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3150" uniqueCount="1513">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3149" uniqueCount="1513">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -12583,9 +12583,6 @@
       <c r="D204" t="s">
         <v>405</v>
       </c>
-      <c r="E204" t="s">
-        <v>537</v>
-      </c>
       <c r="F204" s="2">
         <v>45771</v>
       </c>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-09-24 06:30:37
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3249" uniqueCount="1557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="1557">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -12941,6 +12941,9 @@
       </c>
       <c r="D210" t="s">
         <v>419</v>
+      </c>
+      <c r="E210" t="s">
+        <v>552</v>
       </c>
       <c r="F210" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-09-26 15:34:00
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3537" uniqueCount="1685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3536" uniqueCount="1685">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -14219,9 +14219,6 @@
       </c>
       <c r="D234" t="s">
         <v>456</v>
-      </c>
-      <c r="E234" t="s">
-        <v>602</v>
       </c>
       <c r="F234" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-10 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4332" uniqueCount="2295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4331" uniqueCount="2295">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -16879,9 +16879,6 @@
       </c>
       <c r="D255" t="s">
         <v>956</v>
-      </c>
-      <c r="E255" t="s">
-        <v>1110</v>
       </c>
       <c r="F255" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-11 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4395" uniqueCount="2322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4394" uniqueCount="2322">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17110,9 +17110,6 @@
       </c>
       <c r="D258" t="s">
         <v>968</v>
-      </c>
-      <c r="E258" t="s">
-        <v>1124</v>
       </c>
       <c r="F258" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-12 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4394" uniqueCount="2322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4395" uniqueCount="2322">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17110,6 +17110,9 @@
       </c>
       <c r="D258" t="s">
         <v>968</v>
+      </c>
+      <c r="E258" t="s">
+        <v>1124</v>
       </c>
       <c r="F258" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-12 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4395" uniqueCount="2322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4394" uniqueCount="2322">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17110,9 +17110,6 @@
       </c>
       <c r="D258" t="s">
         <v>968</v>
-      </c>
-      <c r="E258" t="s">
-        <v>1124</v>
       </c>
       <c r="F258" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-13 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4394" uniqueCount="2322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4395" uniqueCount="2322">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17110,6 +17110,9 @@
       </c>
       <c r="D258" t="s">
         <v>968</v>
+      </c>
+      <c r="E258" t="s">
+        <v>1124</v>
       </c>
       <c r="F258" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-17 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4378" uniqueCount="2311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4379" uniqueCount="2311">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -16975,6 +16975,9 @@
       </c>
       <c r="D255" t="s">
         <v>964</v>
+      </c>
+      <c r="E255" t="s">
+        <v>1118</v>
       </c>
       <c r="F255" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-18 00:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4387" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="2316">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17025,6 +17025,9 @@
       </c>
       <c r="D256" t="s">
         <v>966</v>
+      </c>
+      <c r="E256" t="s">
+        <v>1121</v>
       </c>
       <c r="F256" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-18 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4387" uniqueCount="2316">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17025,9 +17025,6 @@
       </c>
       <c r="D256" t="s">
         <v>966</v>
-      </c>
-      <c r="E256" t="s">
-        <v>1121</v>
       </c>
       <c r="F256" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-19 00:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4387" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="2316">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17025,6 +17025,9 @@
       </c>
       <c r="D256" t="s">
         <v>966</v>
+      </c>
+      <c r="E256" t="s">
+        <v>1121</v>
       </c>
       <c r="F256" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-19 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4387" uniqueCount="2316">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17025,9 +17025,6 @@
       </c>
       <c r="D256" t="s">
         <v>966</v>
-      </c>
-      <c r="E256" t="s">
-        <v>1121</v>
       </c>
       <c r="F256" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-20 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4387" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="2316">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17025,6 +17025,9 @@
       </c>
       <c r="D256" t="s">
         <v>966</v>
+      </c>
+      <c r="E256" t="s">
+        <v>1121</v>
       </c>
       <c r="F256" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-24 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4387" uniqueCount="2316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4388" uniqueCount="2316">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -11047,7 +11047,7 @@
         <v>1191</v>
       </c>
       <c r="F77" s="2">
-        <v>45854</v>
+        <v>45985</v>
       </c>
       <c r="G77" t="s">
         <v>1199</v>
@@ -17025,6 +17025,9 @@
       </c>
       <c r="D256" t="s">
         <v>966</v>
+      </c>
+      <c r="E256" t="s">
+        <v>1121</v>
       </c>
       <c r="F256" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-25 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4400" uniqueCount="2321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4399" uniqueCount="2321">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -15557,7 +15557,7 @@
         <v>1205</v>
       </c>
       <c r="H211" t="s">
-        <v>1238</v>
+        <v>1209</v>
       </c>
       <c r="I211" t="s">
         <v>1269</v>
@@ -17078,9 +17078,6 @@
       </c>
       <c r="D257" t="s">
         <v>968</v>
-      </c>
-      <c r="E257" t="s">
-        <v>1123</v>
       </c>
       <c r="F257" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-25 18:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4399" uniqueCount="2321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4400" uniqueCount="2321">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17078,6 +17078,9 @@
       </c>
       <c r="D257" t="s">
         <v>968</v>
+      </c>
+      <c r="E257" t="s">
+        <v>1123</v>
       </c>
       <c r="F257" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-26 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4400" uniqueCount="2321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4399" uniqueCount="2321">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17078,9 +17078,6 @@
       </c>
       <c r="D257" t="s">
         <v>968</v>
-      </c>
-      <c r="E257" t="s">
-        <v>1123</v>
       </c>
       <c r="F257" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-11-28 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4411" uniqueCount="2326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4410" uniqueCount="2326">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17134,9 +17134,6 @@
       </c>
       <c r="D258" t="s">
         <v>970</v>
-      </c>
-      <c r="E258" t="s">
-        <v>1126</v>
       </c>
       <c r="F258" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-03 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4525" uniqueCount="2376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4524" uniqueCount="2376">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -17516,9 +17516,6 @@
       </c>
       <c r="D264" t="s">
         <v>994</v>
-      </c>
-      <c r="E264" t="s">
-        <v>1154</v>
       </c>
       <c r="F264" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-08 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="2467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2467">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18368,9 +18368,6 @@
       </c>
       <c r="D278" t="s">
         <v>1036</v>
-      </c>
-      <c r="E278" t="s">
-        <v>1201</v>
       </c>
       <c r="F278" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-09 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="2467">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18368,6 +18368,9 @@
       </c>
       <c r="D278" t="s">
         <v>1036</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1201</v>
       </c>
       <c r="F278" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-09 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="2467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2467">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18368,9 +18368,6 @@
       </c>
       <c r="D278" t="s">
         <v>1036</v>
-      </c>
-      <c r="E278" t="s">
-        <v>1201</v>
       </c>
       <c r="F278" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-11 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="2466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2466">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18366,9 +18366,6 @@
       </c>
       <c r="D278" t="s">
         <v>1036</v>
-      </c>
-      <c r="E278" t="s">
-        <v>1200</v>
       </c>
       <c r="F278" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-11 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="2466">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18366,6 +18366,9 @@
       </c>
       <c r="D278" t="s">
         <v>1036</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1200</v>
       </c>
       <c r="F278" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-11 18:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="2466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2466">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18366,9 +18366,6 @@
       </c>
       <c r="D278" t="s">
         <v>1036</v>
-      </c>
-      <c r="E278" t="s">
-        <v>1200</v>
       </c>
       <c r="F278" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-12 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4720" uniqueCount="2466">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18366,6 +18366,9 @@
       </c>
       <c r="D278" t="s">
         <v>1036</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1200</v>
       </c>
       <c r="F278" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-19 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4739" uniqueCount="2476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4740" uniqueCount="2476">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18464,6 +18464,9 @@
       </c>
       <c r="D280" t="s">
         <v>1040</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1205</v>
       </c>
       <c r="F280" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-19 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4740" uniqueCount="2476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4739" uniqueCount="2476">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18464,9 +18464,6 @@
       </c>
       <c r="D280" t="s">
         <v>1040</v>
-      </c>
-      <c r="E280" t="s">
-        <v>1205</v>
       </c>
       <c r="F280" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-25 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,9 +18538,6 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
-      </c>
-      <c r="E281" t="s">
-        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-25 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,6 +18538,9 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-26 12:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,9 +18538,6 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
-      </c>
-      <c r="E281" t="s">
-        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-26 18:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,6 +18538,9 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-27 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,9 +18538,6 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
-      </c>
-      <c r="E281" t="s">
-        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-29 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,6 +18538,9 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-29 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,9 +18538,6 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
-      </c>
-      <c r="E281" t="s">
-        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2025-12-30 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,6 +18538,9 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-02 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,9 +18538,6 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
-      </c>
-      <c r="E281" t="s">
-        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-05 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,9 +18538,6 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
-      </c>
-      <c r="E281" t="s">
-        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-06 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,6 +18538,9 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1210</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-06 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -3643,6 +3643,9 @@
     <t>19/03/2025</t>
   </si>
   <si>
+    <t>06/06/2025</t>
+  </si>
+  <si>
     <t>10/10/2024</t>
   </si>
   <si>
@@ -3878,9 +3881,6 @@
   </si>
   <si>
     <t>27/10/2025</t>
-  </si>
-  <si>
-    <t>06/06/2025</t>
   </si>
   <si>
     <t>11/04/2025</t>
@@ -9299,10 +9299,10 @@
         <v>1019</v>
       </c>
       <c r="D3" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="E3" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="F3" s="2">
         <v>45709</v>
@@ -9529,7 +9529,7 @@
         <v>1026</v>
       </c>
       <c r="D10" t="s">
-        <v>1241</v>
+        <v>1242</v>
       </c>
       <c r="E10" t="s">
         <v>1202</v>
@@ -9823,7 +9823,7 @@
         <v>1035</v>
       </c>
       <c r="D19" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="F19" s="2">
         <v>45889</v>
@@ -10696,10 +10696,10 @@
         <v>1058</v>
       </c>
       <c r="D46" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="E46" t="s">
-        <v>1242</v>
+        <v>1243</v>
       </c>
       <c r="F46" s="2">
         <v>45846</v>
@@ -11520,7 +11520,7 @@
         <v>1073</v>
       </c>
       <c r="D71" t="s">
-        <v>1243</v>
+        <v>1244</v>
       </c>
       <c r="F71" s="2">
         <v>45972</v>
@@ -11881,10 +11881,10 @@
         <v>1080</v>
       </c>
       <c r="D82" t="s">
-        <v>1244</v>
+        <v>1245</v>
       </c>
       <c r="E82" t="s">
-        <v>1280</v>
+        <v>1281</v>
       </c>
       <c r="F82" s="2">
         <v>45985</v>
@@ -12117,7 +12117,7 @@
         <v>1084</v>
       </c>
       <c r="D89" t="s">
-        <v>1245</v>
+        <v>1246</v>
       </c>
       <c r="E89" t="s">
         <v>1134</v>
@@ -12190,7 +12190,7 @@
         <v>1086</v>
       </c>
       <c r="D91" t="s">
-        <v>1246</v>
+        <v>1247</v>
       </c>
       <c r="F91" s="2">
         <v>45804</v>
@@ -12356,7 +12356,7 @@
         <v>1019</v>
       </c>
       <c r="D96" t="s">
-        <v>1247</v>
+        <v>1248</v>
       </c>
       <c r="E96" t="s">
         <v>1139</v>
@@ -12525,7 +12525,7 @@
         <v>1090</v>
       </c>
       <c r="E101" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="F101" s="2">
         <v>45727</v>
@@ -12819,7 +12819,7 @@
         <v>1024</v>
       </c>
       <c r="E110" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="F110" s="2">
         <v>45705</v>
@@ -12892,7 +12892,7 @@
         <v>1099</v>
       </c>
       <c r="D112" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="E112" t="s">
         <v>1114</v>
@@ -13122,10 +13122,10 @@
         <v>1104</v>
       </c>
       <c r="D119" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="E119" t="s">
-        <v>1249</v>
+        <v>1250</v>
       </c>
       <c r="F119" s="2">
         <v>45684</v>
@@ -13768,10 +13768,10 @@
         <v>1116</v>
       </c>
       <c r="D139" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="E139" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="F139" s="2">
         <v>45876</v>
@@ -13902,7 +13902,7 @@
         <v>1111</v>
       </c>
       <c r="E143" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="F143" s="2">
         <v>45810</v>
@@ -14004,7 +14004,7 @@
         <v>1045</v>
       </c>
       <c r="E146" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="F146" s="2">
         <v>45894</v>
@@ -14106,10 +14106,10 @@
         <v>1110</v>
       </c>
       <c r="D149" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="E149" t="s">
-        <v>1250</v>
+        <v>1251</v>
       </c>
       <c r="F149" s="2">
         <v>45946</v>
@@ -14176,7 +14176,7 @@
         <v>1121</v>
       </c>
       <c r="D151" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="E151" t="s">
         <v>1062</v>
@@ -14246,7 +14246,7 @@
         <v>1049</v>
       </c>
       <c r="D153" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="F153" s="2">
         <v>45972</v>
@@ -14380,7 +14380,7 @@
         <v>1050</v>
       </c>
       <c r="E157" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
       <c r="F157" s="2">
         <v>45704</v>
@@ -14686,7 +14686,7 @@
         <v>1127</v>
       </c>
       <c r="D166" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="E166" t="s">
         <v>1146</v>
@@ -14762,7 +14762,7 @@
         <v>1129</v>
       </c>
       <c r="D168" t="s">
-        <v>1253</v>
+        <v>1254</v>
       </c>
       <c r="E168" t="s">
         <v>1208</v>
@@ -14838,10 +14838,10 @@
         <v>1131</v>
       </c>
       <c r="D170" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="E170" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="F170" s="2">
         <v>46009</v>
@@ -14876,10 +14876,10 @@
         <v>1132</v>
       </c>
       <c r="D171" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="E171" t="s">
-        <v>1255</v>
+        <v>1256</v>
       </c>
       <c r="F171" s="2">
         <v>45708</v>
@@ -15042,7 +15042,7 @@
         <v>1135</v>
       </c>
       <c r="D176" t="s">
-        <v>1256</v>
+        <v>1257</v>
       </c>
       <c r="E176" t="s">
         <v>1029</v>
@@ -15211,7 +15211,7 @@
         <v>1101</v>
       </c>
       <c r="E181" t="s">
-        <v>1284</v>
+        <v>1285</v>
       </c>
       <c r="F181" s="2">
         <v>45704</v>
@@ -15776,7 +15776,7 @@
         <v>1151</v>
       </c>
       <c r="D198" t="s">
-        <v>1257</v>
+        <v>1258</v>
       </c>
       <c r="F198" s="2">
         <v>45705</v>
@@ -16070,7 +16070,7 @@
         <v>1066</v>
       </c>
       <c r="E207" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="F207" s="2">
         <v>45992</v>
@@ -16137,10 +16137,10 @@
         <v>1154</v>
       </c>
       <c r="D209" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="E209" t="s">
-        <v>1258</v>
+        <v>1259</v>
       </c>
       <c r="F209" s="2">
         <v>45698</v>
@@ -16239,10 +16239,10 @@
         <v>1113</v>
       </c>
       <c r="D212" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="E212" t="s">
-        <v>1259</v>
+        <v>1260</v>
       </c>
       <c r="F212" s="2">
         <v>45880</v>
@@ -16510,10 +16510,10 @@
         <v>1159</v>
       </c>
       <c r="D220" t="s">
-        <v>1260</v>
+        <v>1261</v>
       </c>
       <c r="E220" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="F220" s="2">
         <v>45799</v>
@@ -16915,7 +16915,7 @@
         <v>1164</v>
       </c>
       <c r="D232" t="s">
-        <v>1261</v>
+        <v>1262</v>
       </c>
       <c r="F232" s="2">
         <v>45698</v>
@@ -17014,10 +17014,10 @@
         <v>1165</v>
       </c>
       <c r="D235" t="s">
-        <v>1262</v>
+        <v>1263</v>
       </c>
       <c r="E235" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="F235" s="2">
         <v>45952</v>
@@ -17084,7 +17084,7 @@
         <v>1074</v>
       </c>
       <c r="D237" t="s">
-        <v>1263</v>
+        <v>1264</v>
       </c>
       <c r="E237" t="s">
         <v>1189</v>
@@ -17288,7 +17288,7 @@
         <v>1050</v>
       </c>
       <c r="D243" t="s">
-        <v>1264</v>
+        <v>1265</v>
       </c>
       <c r="F243" s="2">
         <v>45733</v>
@@ -17582,7 +17582,7 @@
         <v>1122</v>
       </c>
       <c r="E252" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="F252" s="2">
         <v>45705</v>
@@ -17617,10 +17617,10 @@
         <v>1061</v>
       </c>
       <c r="D253" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="E253" t="s">
-        <v>1265</v>
+        <v>1266</v>
       </c>
       <c r="F253" s="2">
         <v>45937</v>
@@ -17687,10 +17687,10 @@
         <v>1175</v>
       </c>
       <c r="D255" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="E255" t="s">
-        <v>1266</v>
+        <v>1267</v>
       </c>
       <c r="F255" s="2">
         <v>45734</v>
@@ -17917,10 +17917,10 @@
         <v>1178</v>
       </c>
       <c r="D262" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="E262" t="s">
-        <v>1267</v>
+        <v>1268</v>
       </c>
       <c r="F262" s="2">
         <v>45777</v>
@@ -18539,9 +18539,6 @@
       <c r="D281" t="s">
         <v>1044</v>
       </c>
-      <c r="E281" t="s">
-        <v>1210</v>
-      </c>
       <c r="F281" s="2">
         <v>45771</v>
       </c>
@@ -18735,10 +18732,10 @@
         <v>1094</v>
       </c>
       <c r="D287" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="E287" t="s">
-        <v>1268</v>
+        <v>1269</v>
       </c>
       <c r="F287" s="2">
         <v>45754</v>
@@ -18872,7 +18869,7 @@
         <v>1036</v>
       </c>
       <c r="E291" t="s">
-        <v>1286</v>
+        <v>1287</v>
       </c>
       <c r="F291" s="2">
         <v>45831</v>
@@ -19207,10 +19204,10 @@
         <v>1191</v>
       </c>
       <c r="D301" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="E301" t="s">
-        <v>1269</v>
+        <v>1270</v>
       </c>
       <c r="F301" s="2">
         <v>45699</v>
@@ -19373,7 +19370,7 @@
         <v>1061</v>
       </c>
       <c r="D306" t="s">
-        <v>1248</v>
+        <v>1249</v>
       </c>
       <c r="F306" s="2">
         <v>45972</v>
@@ -19408,7 +19405,7 @@
         <v>1194</v>
       </c>
       <c r="D307" t="s">
-        <v>1270</v>
+        <v>1271</v>
       </c>
       <c r="F307" s="2">
         <v>45853</v>
@@ -19673,7 +19670,7 @@
         <v>1072</v>
       </c>
       <c r="E315" t="s">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="F315" s="2">
         <v>45985</v>
@@ -19804,10 +19801,10 @@
         <v>1171</v>
       </c>
       <c r="D319" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="E319" t="s">
-        <v>1271</v>
+        <v>1272</v>
       </c>
       <c r="F319" s="2">
         <v>45775</v>
@@ -19906,7 +19903,7 @@
         <v>1023</v>
       </c>
       <c r="D322" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="F322" s="2">
         <v>45952</v>
@@ -20264,7 +20261,7 @@
         <v>1091</v>
       </c>
       <c r="E333" t="s">
-        <v>1288</v>
+        <v>1209</v>
       </c>
       <c r="F333" s="2">
         <v>45929</v>
@@ -21027,10 +21024,10 @@
         <v>869</v>
       </c>
       <c r="C356" t="s">
-        <v>1088</v>
+        <v>1209</v>
       </c>
       <c r="F356" s="2">
-        <v>45813</v>
+        <v>46028</v>
       </c>
       <c r="G356" t="s">
         <v>1292</v>
@@ -21126,7 +21123,7 @@
         <v>872</v>
       </c>
       <c r="C359" t="s">
-        <v>1209</v>
+        <v>1210</v>
       </c>
       <c r="F359" s="2">
         <v>45838</v>
@@ -21327,7 +21324,7 @@
         <v>1182</v>
       </c>
       <c r="D365" t="s">
-        <v>1272</v>
+        <v>1273</v>
       </c>
       <c r="F365" s="2">
         <v>45782</v>
@@ -21557,7 +21554,7 @@
         <v>885</v>
       </c>
       <c r="C372" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="F372" s="2">
         <v>45838</v>
@@ -21688,10 +21685,10 @@
         <v>1026</v>
       </c>
       <c r="D376" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="E376" t="s">
-        <v>1283</v>
+        <v>1284</v>
       </c>
       <c r="F376" s="2">
         <v>45992</v>
@@ -21723,7 +21720,7 @@
         <v>890</v>
       </c>
       <c r="C377" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="F377" s="2">
         <v>46010</v>
@@ -21822,7 +21819,7 @@
         <v>893</v>
       </c>
       <c r="C380" t="s">
-        <v>1212</v>
+        <v>1213</v>
       </c>
       <c r="F380" s="2">
         <v>45965</v>
@@ -21921,7 +21918,7 @@
         <v>1121</v>
       </c>
       <c r="D383" t="s">
-        <v>1251</v>
+        <v>1252</v>
       </c>
       <c r="E383" t="s">
         <v>1062</v>
@@ -21959,10 +21956,10 @@
         <v>1087</v>
       </c>
       <c r="D384" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="E384" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="F384" s="2">
         <v>45838</v>
@@ -21994,7 +21991,7 @@
         <v>898</v>
       </c>
       <c r="C385" t="s">
-        <v>1213</v>
+        <v>1214</v>
       </c>
       <c r="F385" s="2">
         <v>45684</v>
@@ -22026,7 +22023,7 @@
         <v>899</v>
       </c>
       <c r="C386" t="s">
-        <v>1214</v>
+        <v>1215</v>
       </c>
       <c r="F386" s="2">
         <v>45743</v>
@@ -22058,10 +22055,10 @@
         <v>900</v>
       </c>
       <c r="C387" t="s">
-        <v>1215</v>
+        <v>1216</v>
       </c>
       <c r="D387" t="s">
-        <v>1274</v>
+        <v>1275</v>
       </c>
       <c r="E387" t="s">
         <v>1050</v>
@@ -22431,13 +22428,13 @@
         <v>911</v>
       </c>
       <c r="C398" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="D398" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="E398" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="F398" s="2">
         <v>45950</v>
@@ -22469,7 +22466,7 @@
         <v>912</v>
       </c>
       <c r="C399" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="F399" s="2">
         <v>45679</v>
@@ -22769,7 +22766,7 @@
         <v>921</v>
       </c>
       <c r="C408" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="F408" s="2">
         <v>45824</v>
@@ -22903,7 +22900,7 @@
         <v>925</v>
       </c>
       <c r="C412" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="F412" s="2">
         <v>45946</v>
@@ -23133,7 +23130,7 @@
         <v>932</v>
       </c>
       <c r="C419" t="s">
-        <v>1210</v>
+        <v>1211</v>
       </c>
       <c r="F419" s="2">
         <v>45722</v>
@@ -23165,7 +23162,7 @@
         <v>933</v>
       </c>
       <c r="C420" t="s">
-        <v>1220</v>
+        <v>1221</v>
       </c>
       <c r="F420" s="2">
         <v>45994</v>
@@ -23232,7 +23229,7 @@
         <v>1060</v>
       </c>
       <c r="D422" t="s">
-        <v>1217</v>
+        <v>1218</v>
       </c>
       <c r="F422" s="2">
         <v>45709</v>
@@ -23296,10 +23293,10 @@
         <v>937</v>
       </c>
       <c r="C424" t="s">
-        <v>1221</v>
+        <v>1222</v>
       </c>
       <c r="D424" t="s">
-        <v>1275</v>
+        <v>1276</v>
       </c>
       <c r="E424" t="s">
         <v>1025</v>
@@ -23398,7 +23395,7 @@
         <v>940</v>
       </c>
       <c r="C427" t="s">
-        <v>1222</v>
+        <v>1223</v>
       </c>
       <c r="F427" s="2">
         <v>45917</v>
@@ -23427,13 +23424,13 @@
         <v>941</v>
       </c>
       <c r="C428" t="s">
-        <v>1223</v>
+        <v>1224</v>
       </c>
       <c r="D428" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="E428" t="s">
-        <v>1276</v>
+        <v>1277</v>
       </c>
       <c r="F428" s="2">
         <v>45670</v>
@@ -23561,7 +23558,7 @@
         <v>945</v>
       </c>
       <c r="C432" t="s">
-        <v>1224</v>
+        <v>1225</v>
       </c>
       <c r="F432" s="2">
         <v>45684</v>
@@ -23771,7 +23768,7 @@
         <v>1056</v>
       </c>
       <c r="E438" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="F438" s="2">
         <v>45799</v>
@@ -23969,13 +23966,13 @@
         <v>957</v>
       </c>
       <c r="C444" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="D444" t="s">
-        <v>1254</v>
+        <v>1255</v>
       </c>
       <c r="E444" t="s">
-        <v>1219</v>
+        <v>1220</v>
       </c>
       <c r="F444" s="2">
         <v>45946</v>
@@ -24007,7 +24004,7 @@
         <v>958</v>
       </c>
       <c r="C445" t="s">
-        <v>1211</v>
+        <v>1212</v>
       </c>
       <c r="F445" s="2">
         <v>45888</v>
@@ -24039,7 +24036,7 @@
         <v>959</v>
       </c>
       <c r="C446" t="s">
-        <v>1226</v>
+        <v>1227</v>
       </c>
       <c r="F446" s="2">
         <v>45709</v>
@@ -24141,7 +24138,7 @@
         <v>962</v>
       </c>
       <c r="C449" t="s">
-        <v>1227</v>
+        <v>1228</v>
       </c>
       <c r="F449" s="2">
         <v>46010</v>
@@ -24403,7 +24400,7 @@
         <v>970</v>
       </c>
       <c r="C457" t="s">
-        <v>1228</v>
+        <v>1229</v>
       </c>
       <c r="F457" s="2">
         <v>45937</v>
@@ -24598,13 +24595,13 @@
         <v>976</v>
       </c>
       <c r="C463" t="s">
-        <v>1229</v>
+        <v>1230</v>
       </c>
       <c r="D463" t="s">
         <v>1042</v>
       </c>
       <c r="E463" t="s">
-        <v>1273</v>
+        <v>1274</v>
       </c>
       <c r="F463" s="2">
         <v>45903</v>
@@ -24668,10 +24665,10 @@
         <v>978</v>
       </c>
       <c r="C465" t="s">
-        <v>1230</v>
+        <v>1231</v>
       </c>
       <c r="D465" t="s">
-        <v>1277</v>
+        <v>1278</v>
       </c>
       <c r="F465" s="2">
         <v>45707</v>
@@ -24770,7 +24767,7 @@
         <v>981</v>
       </c>
       <c r="C468" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="F468" s="2">
         <v>45951</v>
@@ -24802,7 +24799,7 @@
         <v>982</v>
       </c>
       <c r="C469" t="s">
-        <v>1232</v>
+        <v>1233</v>
       </c>
       <c r="F469" s="2">
         <v>45895</v>
@@ -24866,13 +24863,13 @@
         <v>984</v>
       </c>
       <c r="C471" t="s">
-        <v>1233</v>
+        <v>1234</v>
       </c>
       <c r="D471" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="E471" t="s">
-        <v>1216</v>
+        <v>1217</v>
       </c>
       <c r="F471" s="2">
         <v>45946</v>
@@ -24974,7 +24971,7 @@
         <v>987</v>
       </c>
       <c r="C474" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="D474" t="s">
         <v>1050</v>
@@ -25210,7 +25207,7 @@
         <v>994</v>
       </c>
       <c r="C481" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="F481" s="2">
         <v>45925</v>
@@ -25242,7 +25239,7 @@
         <v>995</v>
       </c>
       <c r="C482" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="F482" s="2">
         <v>45684</v>
@@ -25411,7 +25408,7 @@
         <v>1179</v>
       </c>
       <c r="D487" t="s">
-        <v>1278</v>
+        <v>1279</v>
       </c>
       <c r="E487" t="s">
         <v>1150</v>
@@ -25516,7 +25513,7 @@
         <v>1003</v>
       </c>
       <c r="C490" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="F490" s="2">
         <v>45849</v>
@@ -25621,10 +25618,10 @@
         <v>1086</v>
       </c>
       <c r="D493" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="E493" t="s">
-        <v>1279</v>
+        <v>1280</v>
       </c>
       <c r="F493" s="2">
         <v>45740</v>
@@ -25656,7 +25653,7 @@
         <v>1007</v>
       </c>
       <c r="C494" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="F494" s="2">
         <v>45938</v>
@@ -25790,7 +25787,7 @@
         <v>1011</v>
       </c>
       <c r="C498" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="F498" s="2">
         <v>46006</v>
@@ -25886,7 +25883,7 @@
         <v>1014</v>
       </c>
       <c r="C501" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="F501" s="2">
         <v>45762</v>
@@ -25918,7 +25915,7 @@
         <v>1015</v>
       </c>
       <c r="C502" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="F502" s="2">
         <v>45953</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-07 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4757" uniqueCount="2488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4758" uniqueCount="2488">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18538,6 +18538,9 @@
       </c>
       <c r="D281" t="s">
         <v>1044</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1211</v>
       </c>
       <c r="F281" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-08 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4749" uniqueCount="2484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="2484">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18494,9 +18494,6 @@
       </c>
       <c r="D280" t="s">
         <v>1042</v>
-      </c>
-      <c r="E280" t="s">
-        <v>1208</v>
       </c>
       <c r="F280" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-09 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="2484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4749" uniqueCount="2484">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18494,6 +18494,9 @@
       </c>
       <c r="D280" t="s">
         <v>1042</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1208</v>
       </c>
       <c r="F280" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-09 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4749" uniqueCount="2484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="2484">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18494,9 +18494,6 @@
       </c>
       <c r="D280" t="s">
         <v>1042</v>
-      </c>
-      <c r="E280" t="s">
-        <v>1208</v>
       </c>
       <c r="F280" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-09 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4748" uniqueCount="2484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4749" uniqueCount="2484">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -3991,6 +3991,9 @@
     <t>FARMÁCIA</t>
   </si>
   <si>
+    <t>ENGENHARIA QUÍMICA,RECURSOS HÍDRICOS</t>
+  </si>
+  <si>
     <t>ECONOMICIDADE OBRAS,MOBILIDADE E TRANSPORTE</t>
   </si>
   <si>
@@ -4034,9 +4037,6 @@
   </si>
   <si>
     <t>RECURSOS HÍDRICOS,RESÍDUOS SÓLIDOS</t>
-  </si>
-  <si>
-    <t>ENGENHARIA QUÍMICA,RECURSOS HÍDRICOS</t>
   </si>
   <si>
     <t>ASSISTÊNCIA SOCIAL,SAÚDE MENTAL</t>
@@ -15636,7 +15636,7 @@
         <v>1290</v>
       </c>
       <c r="H194" t="s">
-        <v>1307</v>
+        <v>1325</v>
       </c>
       <c r="I194" t="s">
         <v>1383</v>
@@ -16408,7 +16408,7 @@
         <v>1290</v>
       </c>
       <c r="H217" t="s">
-        <v>1325</v>
+        <v>1326</v>
       </c>
       <c r="I217" t="s">
         <v>1440</v>
@@ -16478,7 +16478,7 @@
         <v>1290</v>
       </c>
       <c r="H219" t="s">
-        <v>1326</v>
+        <v>1327</v>
       </c>
       <c r="I219" t="s">
         <v>1374</v>
@@ -16647,7 +16647,7 @@
         <v>1290</v>
       </c>
       <c r="H224" t="s">
-        <v>1327</v>
+        <v>1328</v>
       </c>
       <c r="I224" t="s">
         <v>1423</v>
@@ -17122,7 +17122,7 @@
         <v>1290</v>
       </c>
       <c r="H238" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="I238" t="s">
         <v>1378</v>
@@ -17585,7 +17585,7 @@
         <v>1290</v>
       </c>
       <c r="H252" t="s">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="I252" t="s">
         <v>1430</v>
@@ -17917,7 +17917,7 @@
         <v>1290</v>
       </c>
       <c r="H262" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="I262" t="s">
         <v>1400</v>
@@ -18495,6 +18495,9 @@
       <c r="D280" t="s">
         <v>1042</v>
       </c>
+      <c r="E280" t="s">
+        <v>1208</v>
+      </c>
       <c r="F280" s="2">
         <v>45771</v>
       </c>
@@ -18502,7 +18505,7 @@
         <v>1290</v>
       </c>
       <c r="H280" t="s">
-        <v>1331</v>
+        <v>1332</v>
       </c>
       <c r="I280" t="s">
         <v>1450</v>
@@ -18732,7 +18735,7 @@
         <v>1290</v>
       </c>
       <c r="H287" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="I287" t="s">
         <v>1451</v>
@@ -18904,7 +18907,7 @@
         <v>1290</v>
       </c>
       <c r="H292" t="s">
-        <v>1333</v>
+        <v>1334</v>
       </c>
       <c r="I292" t="s">
         <v>1392</v>
@@ -19172,7 +19175,7 @@
         <v>1290</v>
       </c>
       <c r="H300" t="s">
-        <v>1334</v>
+        <v>1335</v>
       </c>
       <c r="I300" t="s">
         <v>1386</v>
@@ -20092,7 +20095,7 @@
         <v>1290</v>
       </c>
       <c r="H328" t="s">
-        <v>1332</v>
+        <v>1333</v>
       </c>
       <c r="I328" t="s">
         <v>1452</v>
@@ -20386,7 +20389,7 @@
         <v>1290</v>
       </c>
       <c r="H337" t="s">
-        <v>1335</v>
+        <v>1336</v>
       </c>
       <c r="I337" t="s">
         <v>1357</v>
@@ -20893,7 +20896,7 @@
         <v>1291</v>
       </c>
       <c r="H352" t="s">
-        <v>1336</v>
+        <v>1337</v>
       </c>
       <c r="I352" t="s">
         <v>1460</v>
@@ -22096,7 +22099,7 @@
         <v>1290</v>
       </c>
       <c r="H388" t="s">
-        <v>1337</v>
+        <v>1338</v>
       </c>
       <c r="I388" t="s">
         <v>1459</v>
@@ -22565,7 +22568,7 @@
         <v>1290</v>
       </c>
       <c r="H402" t="s">
-        <v>1338</v>
+        <v>1339</v>
       </c>
       <c r="I402" t="s">
         <v>1451</v>
@@ -22597,7 +22600,7 @@
         <v>1290</v>
       </c>
       <c r="H403" t="s">
-        <v>1339</v>
+        <v>1340</v>
       </c>
       <c r="I403" t="s">
         <v>1423</v>
@@ -22667,7 +22670,7 @@
         <v>1290</v>
       </c>
       <c r="H405" t="s">
-        <v>1340</v>
+        <v>1325</v>
       </c>
       <c r="I405" t="s">
         <v>1354</v>
@@ -23663,7 +23666,7 @@
         <v>1290</v>
       </c>
       <c r="H435" t="s">
-        <v>1330</v>
+        <v>1331</v>
       </c>
       <c r="I435" t="s">
         <v>1429</v>
@@ -23899,7 +23902,7 @@
         <v>1290</v>
       </c>
       <c r="H442" t="s">
-        <v>1328</v>
+        <v>1329</v>
       </c>
       <c r="I442" t="s">
         <v>1375</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-15 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4790" uniqueCount="2504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="2504">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18559,6 +18559,9 @@
       </c>
       <c r="D279" t="s">
         <v>1050</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1220</v>
       </c>
       <c r="F279" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-15 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="2504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4790" uniqueCount="2504">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18559,9 +18559,6 @@
       </c>
       <c r="D279" t="s">
         <v>1050</v>
-      </c>
-      <c r="E279" t="s">
-        <v>1220</v>
       </c>
       <c r="F279" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-15 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4790" uniqueCount="2504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="2504">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18559,6 +18559,9 @@
       </c>
       <c r="D279" t="s">
         <v>1050</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1220</v>
       </c>
       <c r="F279" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-19 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="2504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4790" uniqueCount="2504">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18559,9 +18559,6 @@
       </c>
       <c r="D279" t="s">
         <v>1050</v>
-      </c>
-      <c r="E279" t="s">
-        <v>1220</v>
       </c>
       <c r="F279" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-20 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4790" uniqueCount="2504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4791" uniqueCount="2504">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18559,6 +18559,9 @@
       </c>
       <c r="D279" t="s">
         <v>1050</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1220</v>
       </c>
       <c r="F279" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-22 00:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4826" uniqueCount="2522">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4827" uniqueCount="2522">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -18753,6 +18753,9 @@
       </c>
       <c r="D283" t="s">
         <v>1059</v>
+      </c>
+      <c r="E283" t="s">
+        <v>1230</v>
       </c>
       <c r="F283" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-23 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4916" uniqueCount="2565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4917" uniqueCount="2565">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19056,6 +19056,9 @@
       </c>
       <c r="D286" t="s">
         <v>1079</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1262</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-26 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4928" uniqueCount="2569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="2569">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19095,9 +19095,6 @@
       </c>
       <c r="D286" t="s">
         <v>1081</v>
-      </c>
-      <c r="E286" t="s">
-        <v>1264</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-27 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="2569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4928" uniqueCount="2569">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19095,6 +19095,9 @@
       </c>
       <c r="D286" t="s">
         <v>1081</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1264</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-28 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4954" uniqueCount="2581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4955" uniqueCount="2581">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19178,6 +19178,9 @@
       </c>
       <c r="D287" t="s">
         <v>1087</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1271</v>
       </c>
       <c r="F287" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-28 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -3862,7 +3862,7 @@
     <t>19/12/2025</t>
   </si>
   <si>
-    <t>05/10/2025</t>
+    <t>28/01/2026</t>
   </si>
   <si>
     <t>16/09/2025</t>
@@ -25524,7 +25524,7 @@
         <v>1282</v>
       </c>
       <c r="F477" s="2">
-        <v>45937</v>
+        <v>46050</v>
       </c>
       <c r="G477" t="s">
         <v>1345</v>
@@ -27106,10 +27106,10 @@
         <v>1059</v>
       </c>
       <c r="C524" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="F524" s="2">
-        <v>45953</v>
+        <v>46050</v>
       </c>
       <c r="G524" t="s">
         <v>1345</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-29 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4963" uniqueCount="2588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4964" uniqueCount="2588">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19231,6 +19231,9 @@
       </c>
       <c r="D288" t="s">
         <v>1089</v>
+      </c>
+      <c r="E288" t="s">
+        <v>1274</v>
       </c>
       <c r="F288" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-29 12:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4964" uniqueCount="2588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4963" uniqueCount="2588">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19231,9 +19231,6 @@
       </c>
       <c r="D288" t="s">
         <v>1089</v>
-      </c>
-      <c r="E288" t="s">
-        <v>1274</v>
       </c>
       <c r="F288" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-01-31 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4963" uniqueCount="2588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4964" uniqueCount="2588">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19231,6 +19231,9 @@
       </c>
       <c r="D288" t="s">
         <v>1089</v>
+      </c>
+      <c r="E288" t="s">
+        <v>1274</v>
       </c>
       <c r="F288" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-03 12:30:04
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4973" uniqueCount="2592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4972" uniqueCount="2592">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19277,9 +19277,6 @@
       </c>
       <c r="D289" t="s">
         <v>1091</v>
-      </c>
-      <c r="E289" t="s">
-        <v>1276</v>
       </c>
       <c r="F289" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-05 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4926" uniqueCount="2569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4925" uniqueCount="2569">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19104,9 +19104,6 @@
       </c>
       <c r="D286" t="s">
         <v>1081</v>
-      </c>
-      <c r="E286" t="s">
-        <v>1265</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-06 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4926" uniqueCount="2570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="2570">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19110,6 +19110,9 @@
       </c>
       <c r="D286" t="s">
         <v>1081</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1266</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-09 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="2570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4926" uniqueCount="2570">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19110,9 +19110,6 @@
       </c>
       <c r="D286" t="s">
         <v>1081</v>
-      </c>
-      <c r="E286" t="s">
-        <v>1266</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-09 18:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4926" uniqueCount="2570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="2570">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19110,6 +19110,9 @@
       </c>
       <c r="D286" t="s">
         <v>1081</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1266</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-10 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4927" uniqueCount="2570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4926" uniqueCount="2570">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -14250,7 +14250,7 @@
         <v>1190</v>
       </c>
       <c r="F141" s="2">
-        <v>46058</v>
+        <v>46063</v>
       </c>
       <c r="G141" t="s">
         <v>1336</v>
@@ -19110,9 +19110,6 @@
       </c>
       <c r="D286" t="s">
         <v>1081</v>
-      </c>
-      <c r="E286" t="s">
-        <v>1266</v>
       </c>
       <c r="F286" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-12 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4944" uniqueCount="2581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4945" uniqueCount="2581">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19175,6 +19175,9 @@
       </c>
       <c r="D287" t="s">
         <v>1086</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1271</v>
       </c>
       <c r="F287" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-12 12:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4945" uniqueCount="2581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4944" uniqueCount="2581">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19175,9 +19175,6 @@
       </c>
       <c r="D287" t="s">
         <v>1086</v>
-      </c>
-      <c r="E287" t="s">
-        <v>1271</v>
       </c>
       <c r="F287" s="2">
         <v>45771</v>

</xml_diff>

<commit_message>
Add backlog, prod, and saida_sem_it - 2026-02-13 00:30:03
</commit_message>
<xml_diff>
--- a/SaidaSemITGATEAutoCompleto.xlsx
+++ b/SaidaSemITGATEAutoCompleto.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4944" uniqueCount="2581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4945" uniqueCount="2581">
   <si>
     <t>PROCEDIMENTO_SEI</t>
   </si>
@@ -19175,6 +19175,9 @@
       </c>
       <c r="D287" t="s">
         <v>1086</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1271</v>
       </c>
       <c r="F287" s="2">
         <v>45771</v>

</xml_diff>